<commit_message>
Got to outputting markup
</commit_message>
<xml_diff>
--- a/results/140822-W27-1409-2014_Japan_Overall_Championships.xlsx
+++ b/results/140822-W27-1409-2014_Japan_Overall_Championships.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\FpaExcelResultsParser\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F76F6EC-A891-4350-9505-913A3A0A2E98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D611D7D-6E3B-4824-A31E-44FE0D5CDDFB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,6 @@
     <definedName name="Rounds">'[1]New Tournament'!$V$15:$V$19</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -883,6 +882,33 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -892,6 +918,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -903,72 +968,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1364,7 +1363,7 @@
   <dimension ref="B1:R30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1468,10 +1467,10 @@
         <v>20</v>
       </c>
       <c r="C11" s="21"/>
-      <c r="D11" s="22" t="s">
+      <c r="D11" s="22"/>
+      <c r="E11" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="21"/>
       <c r="F11" s="21"/>
       <c r="G11" s="22"/>
       <c r="H11" s="21"/>
@@ -1529,10 +1528,10 @@
       <c r="R12" s="8"/>
     </row>
     <row r="13" spans="2:18" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="58">
+      <c r="B13" s="46">
         <v>1</v>
       </c>
-      <c r="C13" s="61" t="s">
+      <c r="C13" s="49" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="14" t="s">
@@ -1544,17 +1543,17 @@
       <c r="F13" s="13">
         <v>0</v>
       </c>
-      <c r="G13" s="43">
+      <c r="G13" s="52">
         <v>0</v>
       </c>
-      <c r="I13" s="64">
+      <c r="I13" s="55">
         <v>62.5</v>
       </c>
-      <c r="J13" s="49"/>
-      <c r="K13" s="67">
+      <c r="J13" s="58"/>
+      <c r="K13" s="61">
         <v>1</v>
       </c>
-      <c r="L13" s="55">
+      <c r="L13" s="43">
         <v>63.5</v>
       </c>
       <c r="P13" s="5" t="s">
@@ -1566,8 +1565,8 @@
       <c r="R13" s="3"/>
     </row>
     <row r="14" spans="2:18" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="59"/>
-      <c r="C14" s="62"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="50"/>
       <c r="D14" s="12" t="s">
         <v>2</v>
       </c>
@@ -1577,11 +1576,11 @@
       <c r="F14" s="11">
         <v>0</v>
       </c>
-      <c r="G14" s="44"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="68"/>
-      <c r="L14" s="56"/>
+      <c r="G14" s="53"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="62"/>
+      <c r="L14" s="44"/>
       <c r="P14" s="10" t="s">
         <v>26</v>
       </c>
@@ -1591,8 +1590,8 @@
       <c r="R14" s="8"/>
     </row>
     <row r="15" spans="2:18" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="60"/>
-      <c r="C15" s="63"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="51"/>
       <c r="D15" s="7"/>
       <c r="E15" s="6" t="s">
         <v>4</v>
@@ -1600,11 +1599,11 @@
       <c r="F15" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="45"/>
-      <c r="I15" s="66"/>
-      <c r="J15" s="51"/>
-      <c r="K15" s="69"/>
-      <c r="L15" s="57"/>
+      <c r="G15" s="54"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="45"/>
       <c r="P15" s="5" t="s">
         <v>22</v>
       </c>
@@ -1614,10 +1613,10 @@
       <c r="R15" s="3"/>
     </row>
     <row r="16" spans="2:18" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="58">
+      <c r="B16" s="46">
         <v>2</v>
       </c>
-      <c r="C16" s="61" t="s">
+      <c r="C16" s="49" t="s">
         <v>3</v>
       </c>
       <c r="D16" s="14" t="s">
@@ -1629,17 +1628,17 @@
       <c r="F16" s="13">
         <v>0.5</v>
       </c>
-      <c r="G16" s="43">
+      <c r="G16" s="52">
         <v>1</v>
       </c>
-      <c r="I16" s="64">
+      <c r="I16" s="55">
         <v>50</v>
       </c>
-      <c r="J16" s="49"/>
-      <c r="K16" s="67">
+      <c r="J16" s="58"/>
+      <c r="K16" s="61">
         <v>0</v>
       </c>
-      <c r="L16" s="55">
+      <c r="L16" s="43">
         <v>50</v>
       </c>
       <c r="P16" s="10" t="s">
@@ -1651,8 +1650,8 @@
       <c r="R16" s="8"/>
     </row>
     <row r="17" spans="2:18" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="59"/>
-      <c r="C17" s="62"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="50"/>
       <c r="D17" s="12" t="s">
         <v>5</v>
       </c>
@@ -1662,11 +1661,11 @@
       <c r="F17" s="11">
         <v>0.5</v>
       </c>
-      <c r="G17" s="44"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="50"/>
-      <c r="K17" s="68"/>
-      <c r="L17" s="56"/>
+      <c r="G17" s="53"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="44"/>
       <c r="P17" s="5" t="s">
         <v>5</v>
       </c>
@@ -1676,8 +1675,8 @@
       <c r="R17" s="3"/>
     </row>
     <row r="18" spans="2:18" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="60"/>
-      <c r="C18" s="63"/>
+      <c r="B18" s="48"/>
+      <c r="C18" s="51"/>
       <c r="D18" s="7"/>
       <c r="E18" s="6" t="s">
         <v>4</v>
@@ -1685,11 +1684,11 @@
       <c r="F18" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G18" s="45"/>
-      <c r="I18" s="66"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="69"/>
-      <c r="L18" s="57"/>
+      <c r="G18" s="54"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="60"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="45"/>
       <c r="P18" s="10" t="s">
         <v>0</v>
       </c>
@@ -1699,10 +1698,10 @@
       <c r="R18" s="8"/>
     </row>
     <row r="19" spans="2:18" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="58">
+      <c r="B19" s="46">
         <v>3</v>
       </c>
-      <c r="C19" s="61" t="s">
+      <c r="C19" s="49" t="s">
         <v>25</v>
       </c>
       <c r="D19" s="14" t="s">
@@ -1714,17 +1713,17 @@
       <c r="F19" s="13">
         <v>0</v>
       </c>
-      <c r="G19" s="43">
+      <c r="G19" s="52">
         <v>0</v>
       </c>
-      <c r="I19" s="64">
+      <c r="I19" s="55">
         <v>40</v>
       </c>
-      <c r="J19" s="49"/>
-      <c r="K19" s="67">
+      <c r="J19" s="58"/>
+      <c r="K19" s="61">
         <v>0</v>
       </c>
-      <c r="L19" s="55">
+      <c r="L19" s="43">
         <v>40</v>
       </c>
       <c r="P19" s="5" t="s">
@@ -1736,8 +1735,8 @@
       <c r="R19" s="3"/>
     </row>
     <row r="20" spans="2:18" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="59"/>
-      <c r="C20" s="62"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="50"/>
       <c r="D20" s="12" t="s">
         <v>22</v>
       </c>
@@ -1747,11 +1746,11 @@
       <c r="F20" s="11">
         <v>0</v>
       </c>
-      <c r="G20" s="44"/>
-      <c r="I20" s="65"/>
-      <c r="J20" s="50"/>
-      <c r="K20" s="68"/>
-      <c r="L20" s="56"/>
+      <c r="G20" s="53"/>
+      <c r="I20" s="56"/>
+      <c r="J20" s="59"/>
+      <c r="K20" s="62"/>
+      <c r="L20" s="44"/>
       <c r="P20" s="10" t="s">
         <v>1</v>
       </c>
@@ -1761,8 +1760,8 @@
       <c r="R20" s="8"/>
     </row>
     <row r="21" spans="2:18" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="60"/>
-      <c r="C21" s="63"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="51"/>
       <c r="D21" s="7"/>
       <c r="E21" s="6" t="s">
         <v>4</v>
@@ -1770,11 +1769,11 @@
       <c r="F21" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="45"/>
-      <c r="I21" s="66"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="69"/>
-      <c r="L21" s="57"/>
+      <c r="G21" s="54"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="60"/>
+      <c r="K21" s="63"/>
+      <c r="L21" s="45"/>
       <c r="P21" s="5"/>
       <c r="Q21" s="4"/>
       <c r="R21" s="3"/>
@@ -1789,10 +1788,10 @@
         <v>20</v>
       </c>
       <c r="C23" s="21"/>
-      <c r="D23" s="22" t="s">
+      <c r="D23" s="22"/>
+      <c r="E23" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="21"/>
       <c r="F23" s="21"/>
       <c r="G23" s="22" t="s">
         <v>18</v>
@@ -1845,10 +1844,10 @@
       <c r="R24" s="3"/>
     </row>
     <row r="25" spans="2:18" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="58">
+      <c r="B25" s="46">
         <v>1</v>
       </c>
-      <c r="C25" s="61" t="s">
+      <c r="C25" s="49" t="s">
         <v>7</v>
       </c>
       <c r="D25" s="14" t="s">
@@ -1860,15 +1859,15 @@
       <c r="F25" s="13">
         <v>0.5</v>
       </c>
-      <c r="G25" s="43">
+      <c r="G25" s="52">
         <v>1</v>
       </c>
-      <c r="I25" s="46">
+      <c r="I25" s="67">
         <v>35</v>
       </c>
-      <c r="J25" s="49"/>
-      <c r="K25" s="52"/>
-      <c r="L25" s="55">
+      <c r="J25" s="58"/>
+      <c r="K25" s="64"/>
+      <c r="L25" s="43">
         <v>35</v>
       </c>
       <c r="P25" s="10"/>
@@ -1876,8 +1875,8 @@
       <c r="R25" s="8"/>
     </row>
     <row r="26" spans="2:18" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="59"/>
-      <c r="C26" s="62"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="50"/>
       <c r="D26" s="12" t="s">
         <v>5</v>
       </c>
@@ -1887,18 +1886,18 @@
       <c r="F26" s="11">
         <v>0.5</v>
       </c>
-      <c r="G26" s="44"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="50"/>
-      <c r="K26" s="53"/>
-      <c r="L26" s="56"/>
+      <c r="G26" s="53"/>
+      <c r="I26" s="68"/>
+      <c r="J26" s="59"/>
+      <c r="K26" s="65"/>
+      <c r="L26" s="44"/>
       <c r="P26" s="5"/>
       <c r="Q26" s="4"/>
       <c r="R26" s="3"/>
     </row>
     <row r="27" spans="2:18" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="60"/>
-      <c r="C27" s="63"/>
+      <c r="B27" s="48"/>
+      <c r="C27" s="51"/>
       <c r="D27" s="7"/>
       <c r="E27" s="6" t="s">
         <v>4</v>
@@ -1906,20 +1905,20 @@
       <c r="F27" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G27" s="45"/>
-      <c r="I27" s="48"/>
-      <c r="J27" s="51"/>
-      <c r="K27" s="54"/>
-      <c r="L27" s="57"/>
+      <c r="G27" s="54"/>
+      <c r="I27" s="69"/>
+      <c r="J27" s="60"/>
+      <c r="K27" s="66"/>
+      <c r="L27" s="45"/>
       <c r="P27" s="10"/>
       <c r="Q27" s="9"/>
       <c r="R27" s="8"/>
     </row>
     <row r="28" spans="2:18" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="58">
+      <c r="B28" s="46">
         <v>2</v>
       </c>
-      <c r="C28" s="61" t="s">
+      <c r="C28" s="49" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="14" t="s">
@@ -1931,15 +1930,15 @@
       <c r="F28" s="13">
         <v>0</v>
       </c>
-      <c r="G28" s="43">
+      <c r="G28" s="52">
         <v>0</v>
       </c>
-      <c r="I28" s="46">
+      <c r="I28" s="67">
         <v>30</v>
       </c>
-      <c r="J28" s="49"/>
-      <c r="K28" s="52"/>
-      <c r="L28" s="55">
+      <c r="J28" s="58"/>
+      <c r="K28" s="64"/>
+      <c r="L28" s="43">
         <v>30</v>
       </c>
       <c r="P28" s="5"/>
@@ -1947,8 +1946,8 @@
       <c r="R28" s="3"/>
     </row>
     <row r="29" spans="2:18" ht="11.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="59"/>
-      <c r="C29" s="62"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="50"/>
       <c r="D29" s="12" t="s">
         <v>1</v>
       </c>
@@ -1958,18 +1957,18 @@
       <c r="F29" s="11">
         <v>0</v>
       </c>
-      <c r="G29" s="44"/>
-      <c r="I29" s="47"/>
-      <c r="J29" s="50"/>
-      <c r="K29" s="53"/>
-      <c r="L29" s="56"/>
+      <c r="G29" s="53"/>
+      <c r="I29" s="68"/>
+      <c r="J29" s="59"/>
+      <c r="K29" s="65"/>
+      <c r="L29" s="44"/>
       <c r="P29" s="10"/>
       <c r="Q29" s="9"/>
       <c r="R29" s="8"/>
     </row>
     <row r="30" spans="2:18" ht="11.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="60"/>
-      <c r="C30" s="63"/>
+      <c r="B30" s="48"/>
+      <c r="C30" s="51"/>
       <c r="D30" s="7" t="s">
         <v>0</v>
       </c>
@@ -1979,31 +1978,22 @@
       <c r="F30" s="6">
         <v>0</v>
       </c>
-      <c r="G30" s="45"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="51"/>
-      <c r="K30" s="54"/>
-      <c r="L30" s="57"/>
+      <c r="G30" s="54"/>
+      <c r="I30" s="69"/>
+      <c r="J30" s="60"/>
+      <c r="K30" s="66"/>
+      <c r="L30" s="45"/>
       <c r="P30" s="5"/>
       <c r="Q30" s="4"/>
       <c r="R30" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="L13:L15"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="G16:G18"/>
-    <mergeCell ref="I16:I18"/>
-    <mergeCell ref="J16:J18"/>
-    <mergeCell ref="K16:K18"/>
-    <mergeCell ref="L16:L18"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="G13:G15"/>
-    <mergeCell ref="I13:I15"/>
-    <mergeCell ref="J13:J15"/>
-    <mergeCell ref="K13:K15"/>
+    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="J25:J27"/>
+    <mergeCell ref="K25:K27"/>
+    <mergeCell ref="L25:L27"/>
     <mergeCell ref="K28:K30"/>
     <mergeCell ref="L28:L30"/>
     <mergeCell ref="B25:B27"/>
@@ -2020,11 +2010,20 @@
     <mergeCell ref="G28:G30"/>
     <mergeCell ref="I28:I30"/>
     <mergeCell ref="J28:J30"/>
-    <mergeCell ref="G25:G27"/>
-    <mergeCell ref="I25:I27"/>
-    <mergeCell ref="J25:J27"/>
-    <mergeCell ref="K25:K27"/>
-    <mergeCell ref="L25:L27"/>
+    <mergeCell ref="L13:L15"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="G16:G18"/>
+    <mergeCell ref="I16:I18"/>
+    <mergeCell ref="J16:J18"/>
+    <mergeCell ref="K16:K18"/>
+    <mergeCell ref="L16:L18"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="I13:I15"/>
+    <mergeCell ref="J13:J15"/>
+    <mergeCell ref="K13:K15"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" promptTitle="Choose Category" sqref="D6" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -2033,7 +2032,7 @@
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B11 B23" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>Divisions</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D11 D23" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" sqref="D11:E11 D23:E23" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>Rounds</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G11 G23" xr:uid="{00000000-0002-0000-0000-000003000000}">

</xml_diff>